<commit_message>
move remaining plot and interpretation chores to kafka
also:

+ modifications to CMS driven measurements for June 2025 experiment
+ better bsui <-> qs communication via zmq or https. thx to Phil
+ take more care not to do things that qs cannot due to being on a different machine
+ use slit_height scan rather than mirror for moving to XRD mode
+ use finalize_wrapper for ga.auto_align
+ move peak, step, and rectangle plotting and interpretation to kafka client
+ abstracted scan interpretation tasks to prepare_alignment_scan
+ communicate scan interpretation back through redis
+ fetch_peak_position_via_redis
+ added a verify limits function before starting change_edge()
+ lookup table corrections for XRD mode
</commit_message>
<xml_diff>
--- a/startup/lookup_table/Modes.xlsx
+++ b/startup/lookup_table/Modes.xlsx
@@ -11828,14 +11828,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="O58" activeCellId="0" sqref="O58"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="T55" activeCellId="0" sqref="T55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14828,7 +14828,7 @@
         <v>141529</v>
       </c>
       <c r="T54" s="57" t="n">
-        <v>58.501</v>
+        <v>58.67</v>
       </c>
       <c r="U54" s="28" t="n">
         <v>497477</v>
@@ -14982,7 +14982,7 @@
       <c r="R56" s="26"/>
       <c r="S56" s="26"/>
       <c r="T56" s="55" t="n">
-        <v>139.4</v>
+        <v>141.1</v>
       </c>
       <c r="U56" s="25" t="n">
         <v>10530029</v>
@@ -15596,7 +15596,7 @@
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="O58 C27"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17119,7 +17119,7 @@
       </c>
       <c r="F30" s="103" t="n">
         <f aca="false">'Modes A-F'!T54</f>
-        <v>58.501</v>
+        <v>58.67</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -17170,10 +17170,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="O58 G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17354,10 +17354,10 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="O58 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.96"/>
@@ -17930,10 +17930,10 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O58 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="102" min="2" style="0" width="11.96"/>
@@ -24002,10 +24002,10 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="O58 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>